<commit_message>
write teaching unit (not finished)
</commit_message>
<xml_diff>
--- a/planning/TestParser.xlsx
+++ b/planning/TestParser.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Teachning unit name</t>
   </si>
@@ -59,139 +59,118 @@
     <t>Suivi en CRL (variable selon test d'entrée)</t>
   </si>
   <si>
-    <t>Probabilite et statistiques</t>
-  </si>
-  <si>
-    <t>Probabilités</t>
-  </si>
-  <si>
-    <t>J.C. Bourgoin</t>
-  </si>
-  <si>
-    <t>Statistiques</t>
-  </si>
-  <si>
-    <t>Ch Lenté</t>
-  </si>
-  <si>
-    <t>M.Slimane</t>
-  </si>
-  <si>
-    <t>Conception et programmation objet : mise en œuvre c++</t>
-  </si>
-  <si>
-    <t>Algorithmique Objet</t>
-  </si>
-  <si>
-    <t>V. T'Kindt</t>
+    <t>Outils mathematiques pour l'ingenieur</t>
+  </si>
+  <si>
+    <t>Outils mathématiques pour l'ingénieur</t>
+  </si>
+  <si>
+    <t>Ch. Lenté</t>
+  </si>
+  <si>
+    <t>Programmation imperative et mise en œuvre</t>
+  </si>
+  <si>
+    <t>Langage C</t>
   </si>
   <si>
     <t>ATER2</t>
   </si>
   <si>
-    <t>Programmation orientée objet : C++</t>
-  </si>
-  <si>
-    <t>projet tutoré C++</t>
-  </si>
-  <si>
-    <t>Transmission de l'information et reseaux</t>
-  </si>
-  <si>
-    <t>Transmission de l'information</t>
-  </si>
-  <si>
-    <t>H. Cardot</t>
-  </si>
-  <si>
-    <t>Réseaux</t>
-  </si>
-  <si>
-    <t>R. Ravaux</t>
-  </si>
-  <si>
-    <t>Mostapha Darwich</t>
-  </si>
-  <si>
-    <t>Systeme et parallelisme</t>
-  </si>
-  <si>
-    <t>Outil pour la synchronisation</t>
-  </si>
-  <si>
-    <t>J. Mendoza</t>
-  </si>
-  <si>
-    <t>Programmation multi-cœur et GPU</t>
-  </si>
-  <si>
-    <t>P. Martineau</t>
-  </si>
-  <si>
-    <t>Systèmes répartis</t>
+    <t>M. Darwich</t>
+  </si>
+  <si>
+    <t>Compilation</t>
+  </si>
+  <si>
+    <t>N. Monmarché</t>
+  </si>
+  <si>
+    <t>Projet tutoré 1</t>
+  </si>
+  <si>
+    <t>R. Bocquillon</t>
+  </si>
+  <si>
+    <t>H. Cherni</t>
+  </si>
+  <si>
+    <t>Conception et utilisation de bases de donnees</t>
+  </si>
+  <si>
+    <t>Conception et utilisation de bases de donnée</t>
+  </si>
+  <si>
+    <t>C.Tacquard</t>
+  </si>
+  <si>
+    <t>M. Martineau</t>
+  </si>
+  <si>
+    <t>Principes fondamentaux et mise en oeuvre des se</t>
+  </si>
+  <si>
+    <t>Architecture des ordinateurs et principes fondamentaux des SE</t>
   </si>
   <si>
     <t>M. Delalandre</t>
   </si>
   <si>
-    <t>M. Bollaert</t>
-  </si>
-  <si>
-    <t>Conception et programmation objet : mise en œuvre java</t>
-  </si>
-  <si>
-    <t>Modélisation orientée objet (UML)</t>
-  </si>
-  <si>
-    <t>Programmation orientée objet : Java</t>
-  </si>
-  <si>
-    <t>C. Esswein</t>
-  </si>
-  <si>
-    <t>C Gatay/F.Chauveau</t>
-  </si>
-  <si>
-    <t>projet tutoré java</t>
-  </si>
-  <si>
-    <t>Shejs2 et anglais2</t>
-  </si>
-  <si>
-    <t>Anglais spécialité informatique</t>
-  </si>
-  <si>
-    <t>Ingénieur dans la société : Epistémologie</t>
-  </si>
-  <si>
-    <t>Gr SHEJS</t>
-  </si>
-  <si>
-    <t>Ingénieur dans la société : Développement durable</t>
-  </si>
-  <si>
-    <t>Qualité de vie au travail - introduction</t>
-  </si>
-  <si>
-    <t>Carsat aract</t>
-  </si>
-  <si>
-    <t>Droit de l'informatique *</t>
-  </si>
-  <si>
-    <t>V. Leperlier Roy</t>
+    <t>P. Makris</t>
+  </si>
+  <si>
+    <t>Illustration d'un SE : Unix</t>
+  </si>
+  <si>
+    <t>J Mendoza</t>
+  </si>
+  <si>
+    <t>Genie logiciel et mise en œuvre</t>
+  </si>
+  <si>
+    <t>Algorithmique</t>
+  </si>
+  <si>
+    <t>G. Venturini</t>
+  </si>
+  <si>
+    <t>Introduction au génie logiciel</t>
+  </si>
+  <si>
+    <t>N. Ragot</t>
+  </si>
+  <si>
+    <t>Projet tutoré 2</t>
+  </si>
+  <si>
+    <t>N. Monmarché/P. Gaucher/Y. Kergosien</t>
+  </si>
+  <si>
+    <t>Shejs1 et anglais1</t>
+  </si>
+  <si>
+    <t>Anglais scientifique</t>
+  </si>
+  <si>
+    <t>BV Langue - Mutualisé avec GAE</t>
+  </si>
+  <si>
+    <t>Ingénieur dans la société : Interculturalité</t>
+  </si>
+  <si>
+    <t>S. Amary</t>
+  </si>
+  <si>
+    <t>Environnement économique de l'entreprise : Jeux création entreprise</t>
+  </si>
+  <si>
+    <t>I. Calmé et …  (IAE)</t>
   </si>
   <si>
     <t>Management de Projet et Conduite Participative</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>Stage  annee 3</t>
-  </si>
-  <si>
-    <t>Stage découverte entreprise (4 semaines minimum)</t>
   </si>
 </sst>
 </file>
@@ -199,453 +178,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="331">
+  <fonts count="243">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -1878,7 +1417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="331">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
@@ -2604,270 +2143,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="242" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="243" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="244" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="245" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="246" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="247" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="248" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="249" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="250" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="251" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="252" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="253" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="254" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="255" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="256" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="257" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="258" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="259" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="260" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="261" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="262" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="263" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="264" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="265" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="266" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="267" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="268" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="269" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="270" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="271" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="272" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="273" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="274" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="275" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="276" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="277" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="278" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="279" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="280" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="281" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="282" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="283" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="284" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="285" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="286" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="287" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="288" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="289" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="290" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="291" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="292" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="293" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="294" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="295" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="296" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="297" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="298" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="299" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="300" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="301" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="302" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="303" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="304" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="305" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="306" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="307" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="308" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="309" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="310" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="311" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="312" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="313" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="314" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="315" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="316" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="317" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="318" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="319" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="320" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="321" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="322" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="323" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="324" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="325" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="326" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="327" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="328" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="329" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="330" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2876,7 +2151,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:M32"/>
+  <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2937,7 +2212,7 @@
         <v>0.0</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I3" s="8" t="n">
         <v>0.0</v>
@@ -2995,13 +2270,13 @@
         <v>16</v>
       </c>
       <c r="D5" s="25" t="n">
-        <v>18.0</v>
+        <v>24.0</v>
       </c>
       <c r="E5" s="26" t="n">
-        <v>8.0</v>
+        <v>24.0</v>
       </c>
       <c r="F5" s="27" t="n">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
       <c r="G5" s="28" t="n">
         <v>0.0</v>
@@ -3010,7 +2285,7 @@
         <v>1.0</v>
       </c>
       <c r="I5" s="30" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J5" s="31" t="n">
         <v>0.0</v>
@@ -3024,19 +2299,19 @@
     </row>
     <row r="6">
       <c r="B6" s="34" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="36" t="n">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="E6" s="37" t="n">
         <v>0.0</v>
       </c>
       <c r="F6" s="38" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="G6" s="39" t="n">
         <v>0.0</v>
@@ -3054,24 +2329,24 @@
         <v>0.0</v>
       </c>
       <c r="L6" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="45" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="47" t="n">
-        <v>18.0</v>
+        <v>0.0</v>
       </c>
       <c r="E7" s="48" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="F7" s="49" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="G7" s="50" t="n">
         <v>0.0</v>
@@ -3089,12 +2364,12 @@
         <v>0.0</v>
       </c>
       <c r="L7" s="55" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="56" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="57" t="s">
         <v>22</v>
@@ -3103,10 +2378,10 @@
         <v>8.0</v>
       </c>
       <c r="E8" s="59" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="F8" s="60" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="G8" s="61" t="n">
         <v>0.0</v>
@@ -3129,115 +2404,115 @@
     </row>
     <row r="9">
       <c r="B9" s="67" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" s="69" t="n">
         <v>0.0</v>
       </c>
       <c r="E9" s="70" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="F9" s="71" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="G9" s="72" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="H9" s="73" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I9" s="74" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J9" s="75" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="K9" s="76" t="n">
         <v>0.0</v>
       </c>
       <c r="L9" s="77" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="78" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="80" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" s="81" t="n">
         <v>0.0</v>
       </c>
       <c r="F10" s="82" t="n">
-        <v>8.0</v>
+        <v>25.0</v>
       </c>
       <c r="G10" s="83" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="H10" s="84" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I10" s="85" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J10" s="86" t="n">
         <v>0.0</v>
       </c>
       <c r="K10" s="87" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="L10" s="88" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="89" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C11" s="90" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D11" s="91" t="n">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
       <c r="E11" s="92" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="F11" s="93" t="n">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
       <c r="G11" s="94" t="n">
         <v>0.0</v>
       </c>
       <c r="H11" s="95" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I11" s="96" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J11" s="97" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="K11" s="98" t="n">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
       <c r="L11" s="99" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="100" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C12" s="101" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12" s="102" t="n">
         <v>0.0</v>
@@ -3246,10 +2521,10 @@
         <v>0.0</v>
       </c>
       <c r="F12" s="104" t="n">
-        <v>25.0</v>
+        <v>12.0</v>
       </c>
       <c r="G12" s="105" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="H12" s="106" t="n">
         <v>1.0</v>
@@ -3261,27 +2536,27 @@
         <v>0.0</v>
       </c>
       <c r="K12" s="109" t="n">
-        <v>25.0</v>
+        <v>12.0</v>
       </c>
       <c r="L12" s="110" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="111" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C13" s="112" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D13" s="113" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
       <c r="E13" s="114" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="F13" s="115" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="G13" s="116" t="n">
         <v>0.0</v>
@@ -3299,59 +2574,59 @@
         <v>0.0</v>
       </c>
       <c r="L13" s="121" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="122" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C14" s="123" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" s="124" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="E14" s="125" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="126" t="n">
         <v>2.0</v>
       </c>
-      <c r="F14" s="126" t="n">
-        <v>0.0</v>
-      </c>
       <c r="G14" s="127" t="n">
         <v>0.0</v>
       </c>
       <c r="H14" s="128" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I14" s="129" t="n">
         <v>1.0</v>
       </c>
       <c r="J14" s="130" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K14" s="131" t="n">
         <v>0.0</v>
       </c>
       <c r="L14" s="132" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="133" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C15" s="134" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D15" s="135" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="E15" s="136" t="n">
         <v>0.0</v>
       </c>
       <c r="F15" s="137" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="G15" s="138" t="n">
         <v>0.0</v>
@@ -3360,33 +2635,33 @@
         <v>1.0</v>
       </c>
       <c r="I15" s="140" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J15" s="141" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="K15" s="142" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="L15" s="143" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="144" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" s="145" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D16" s="146" t="n">
         <v>0.0</v>
       </c>
       <c r="E16" s="147" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F16" s="148" t="n">
-        <v>6.0</v>
+        <v>22.0</v>
       </c>
       <c r="G16" s="149" t="n">
         <v>0.0</v>
@@ -3395,33 +2670,33 @@
         <v>1.0</v>
       </c>
       <c r="I16" s="151" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J16" s="152" t="n">
         <v>0.0</v>
       </c>
       <c r="K16" s="153" t="n">
-        <v>0.0</v>
+        <v>22.0</v>
       </c>
       <c r="L16" s="154" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="155" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C17" s="156" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D17" s="157" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="E17" s="158" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F17" s="159" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G17" s="160" t="n">
         <v>0.0</v>
@@ -3433,30 +2708,30 @@
         <v>0.0</v>
       </c>
       <c r="J17" s="163" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="K17" s="164" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="L17" s="165" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="166" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C18" s="167" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D18" s="168" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="E18" s="169" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="F18" s="170" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G18" s="171" t="n">
         <v>0.0</v>
@@ -3468,30 +2743,30 @@
         <v>0.0</v>
       </c>
       <c r="J18" s="174" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="K18" s="175" t="n">
         <v>0.0</v>
       </c>
       <c r="L18" s="176" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="177" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C19" s="178" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D19" s="179" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="E19" s="180" t="n">
         <v>0.0</v>
       </c>
       <c r="F19" s="181" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="G19" s="182" t="n">
         <v>0.0</v>
@@ -3506,30 +2781,30 @@
         <v>0.0</v>
       </c>
       <c r="K19" s="186" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="L19" s="187" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="188" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C20" s="189" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D20" s="190" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E20" s="191" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F20" s="192" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="G20" s="193" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="H20" s="194" t="n">
         <v>1.0</v>
@@ -3538,27 +2813,27 @@
         <v>0.0</v>
       </c>
       <c r="J20" s="196" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="K20" s="197" t="n">
         <v>0.0</v>
       </c>
       <c r="L20" s="198" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="199" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C21" s="200" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D21" s="201" t="n">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="E21" s="202" t="n">
-        <v>8.0</v>
+        <v>40.0</v>
       </c>
       <c r="F21" s="203" t="n">
         <v>0.0</v>
@@ -3567,7 +2842,7 @@
         <v>0.0</v>
       </c>
       <c r="H21" s="205" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I21" s="206" t="n">
         <v>1.0</v>
@@ -3579,21 +2854,21 @@
         <v>0.0</v>
       </c>
       <c r="L21" s="209" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="210" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C22" s="211" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D22" s="212" t="n">
         <v>0.0</v>
       </c>
       <c r="E22" s="213" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="F22" s="214" t="n">
         <v>0.0</v>
@@ -3602,33 +2877,33 @@
         <v>0.0</v>
       </c>
       <c r="H22" s="216" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I22" s="217" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J22" s="218" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="K22" s="219" t="n">
         <v>0.0</v>
       </c>
       <c r="L22" s="220" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="221" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C23" s="222" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D23" s="223" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="E23" s="224" t="n">
-        <v>6.0</v>
+        <v>14.0</v>
       </c>
       <c r="F23" s="225" t="n">
         <v>0.0</v>
@@ -3649,30 +2924,30 @@
         <v>0.0</v>
       </c>
       <c r="L23" s="231" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="232" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C24" s="233" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D24" s="234" t="n">
         <v>0.0</v>
       </c>
       <c r="E24" s="235" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F24" s="236" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G24" s="237" t="n">
         <v>0.0</v>
       </c>
       <c r="H24" s="238" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I24" s="239" t="n">
         <v>0.0</v>
@@ -3684,305 +2959,23 @@
         <v>0.0</v>
       </c>
       <c r="L24" s="242" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="243" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="244" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="245" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E25" s="246" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F25" s="247" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="G25" s="248" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H25" s="249" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I25" s="250" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J25" s="251" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K25" s="252" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L25" s="253" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="254" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="255" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="256" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E26" s="257" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="F26" s="258" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G26" s="259" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H26" s="260" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I26" s="261" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J26" s="262" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K26" s="263" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L26" s="264" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="265" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="266" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="267" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="E27" s="268" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F27" s="269" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G27" s="270" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H27" s="271" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I27" s="272" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J27" s="273" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K27" s="274" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L27" s="275" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="276" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="277" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="278" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="E28" s="279" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F28" s="280" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G28" s="281" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H28" s="282" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I28" s="283" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J28" s="284" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K28" s="285" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L28" s="286" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="287" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="288" t="s">
         <v>52</v>
-      </c>
-      <c r="D29" s="289" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E29" s="290" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="F29" s="291" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G29" s="292" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H29" s="293" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I29" s="294" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J29" s="295" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K29" s="296" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L29" s="297" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" s="298" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="299" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="300" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="E30" s="301" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F30" s="302" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G30" s="303" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H30" s="304" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I30" s="305" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J30" s="306" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K30" s="307" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L30" s="308" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="309" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="310" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="311" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E31" s="312" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F31" s="313" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G31" s="314" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H31" s="315" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I31" s="316" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J31" s="317" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K31" s="318" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L31" s="319" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" s="320" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="321" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="322" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E32" s="323" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F32" s="324" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G32" s="325" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H32" s="326" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I32" s="327" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J32" s="328" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K32" s="329" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L32" s="330" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
     <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C17:C18"/>
     <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="B21:B24"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>